<commit_message>
fix 2 bugs, matches dada results
</commit_message>
<xml_diff>
--- a/Example Parameters.xlsx
+++ b/Example Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1-9BdNIiT7Zve61xm0MKrEiBMif4tQ21K\Dads Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dads Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD6FF8-BB79-475E-B214-AFEBED8834B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6493288D-C2E6-4270-84CF-105CF842BEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="15630" xr2:uid="{6815C413-B74D-4932-A894-0C3596BD82BE}"/>
+    <workbookView xWindow="768" yWindow="624" windowWidth="21600" windowHeight="11328" xr2:uid="{6815C413-B74D-4932-A894-0C3596BD82BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -510,20 +507,20 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -554,7 +551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -580,7 +577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -594,7 +591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -605,7 +602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -622,7 +619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -648,7 +645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -674,7 +671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -694,7 +691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -714,7 +711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -723,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -731,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -757,7 +754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -783,7 +780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -797,7 +794,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>

</xml_diff>